<commit_message>
Updated Manual Data Entry
</commit_message>
<xml_diff>
--- a/scr/main/resources/data/Data.xlsx
+++ b/scr/main/resources/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecha\Documents\GitHub\Invited-Meeting-Scheduler\scr\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08290EDE-A2F0-48A6-8E17-528B4D090ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B56BACF-AD77-4DE1-B1EB-F2B73EB20AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F80A9F9-5585-4065-BFAC-5B8001948D72}"/>
   </bookViews>
@@ -32,6 +32,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>SMCS</t>
+  </si>
+  <si>
+    <t>Humanities</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,14 +407,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E2F09D-A6EF-4BA7-A519-8563A1C005D0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added a method to create the Schedules
</commit_message>
<xml_diff>
--- a/scr/main/resources/data/Data.xlsx
+++ b/scr/main/resources/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecha\Documents\GitHub\Invited-Meeting-Scheduler\scr\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9B23A-5B98-4FCE-93EE-49873CEDF24B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1417EA9-6B77-4A9E-957F-B899B767903E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F80A9F9-5585-4065-BFAC-5B8001948D72}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25080" windowHeight="11385" activeTab="1" xr2:uid="{3F80A9F9-5585-4065-BFAC-5B8001948D72}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,45 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>ROT</t>
+  </si>
+  <si>
+    <t>ROT1</t>
+  </si>
+  <si>
+    <t>ROT2</t>
+  </si>
+  <si>
+    <t>ROT3</t>
+  </si>
+  <si>
+    <t>ROT4</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
@@ -423,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E2F09D-A6EF-4BA7-A519-8563A1C005D0}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,12 +544,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39036EF1-7472-42F9-BE21-BF99A6FD70B5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>